<commit_message>
"No474. Ones and Zeroes finished"
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NutsWorkFile\我的坚果云\Leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA28474-B241-4A50-8193-F3FD82EB5136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55697430-9811-4C0C-97C8-ED8F4D252E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -825,6 +825,17 @@
   </si>
   <si>
     <t>完全背包问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>474. Ones and Zeroes</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/ones-and-zeroes/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>背包体积约束条件有两个，dp数组多一个维度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1447,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2091,6 +2102,32 @@
       </c>
       <c r="G27" s="28" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A28" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="20">
+        <v>44506</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" s="42" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2127,8 +2164,9 @@
     <hyperlink ref="C25" r:id="rId23" xr:uid="{9D35FEA0-1AA5-47A8-BAA4-E9771260EB8C}"/>
     <hyperlink ref="C26" r:id="rId24" xr:uid="{97F3E1F3-FFCC-4707-96EE-48AC8DC1E40C}"/>
     <hyperlink ref="C27" r:id="rId25" xr:uid="{BC25EE82-9C5F-46E0-81DD-DFF14CDF4B5F}"/>
+    <hyperlink ref="C28" r:id="rId26" xr:uid="{6BF277A1-4D21-48E4-BB89-322C6423FE35}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
474. Ones and Zeroes finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55697430-9811-4C0C-97C8-ED8F4D252E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62544303-8FF3-4192-8DD7-68BF835E88DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -1461,7 +1461,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
No650. 2 Keys Keyboard finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62544303-8FF3-4192-8DD7-68BF835E88DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3296CE4-F215-4938-9149-A3D11BCFAC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="106">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -836,6 +836,22 @@
   </si>
   <si>
     <t>背包体积约束条件有两个，dp数组多一个维度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>650. 2 Keys Keyboard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/2-keys-keyboard/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串编辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>转换成递归找最小因数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1458,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2127,6 +2143,32 @@
         <v>37</v>
       </c>
       <c r="H28" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A29" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="20">
+        <v>44507</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="42" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2165,8 +2207,9 @@
     <hyperlink ref="C26" r:id="rId24" xr:uid="{97F3E1F3-FFCC-4707-96EE-48AC8DC1E40C}"/>
     <hyperlink ref="C27" r:id="rId25" xr:uid="{BC25EE82-9C5F-46E0-81DD-DFF14CDF4B5F}"/>
     <hyperlink ref="C28" r:id="rId26" xr:uid="{6BF277A1-4D21-48E4-BB89-322C6423FE35}"/>
+    <hyperlink ref="C29" r:id="rId27" xr:uid="{DB5A1B9B-6195-4ED2-AE10-F30A38579E65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"No53. Maximum Subarray finished"
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3296CE4-F215-4938-9149-A3D11BCFAC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7FFD7E-348A-42BF-BD87-A2A5163C20D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -1477,7 +1477,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
N053. Maximum Subarray finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7FFD7E-348A-42BF-BD87-A2A5163C20D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F643D1-F18A-4CB0-8649-F3780B844FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="110">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -852,6 +852,34 @@
   </si>
   <si>
     <t>转换成递归找最小因数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>53. Maximum Subarray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-subarray/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>dp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>含义为当前元素为末尾的子序列最大和；可以空间压缩；另设一变量更新遍历过程中所有dp的最大值；</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态规划；最大连续子序列和</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1026,7 +1054,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1158,6 +1186,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1474,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2170,6 +2201,29 @@
       </c>
       <c r="H29" s="42" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A30" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="6">
+        <v>44508</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2208,8 +2262,9 @@
     <hyperlink ref="C27" r:id="rId25" xr:uid="{BC25EE82-9C5F-46E0-81DD-DFF14CDF4B5F}"/>
     <hyperlink ref="C28" r:id="rId26" xr:uid="{6BF277A1-4D21-48E4-BB89-322C6423FE35}"/>
     <hyperlink ref="C29" r:id="rId27" xr:uid="{DB5A1B9B-6195-4ED2-AE10-F30A38579E65}"/>
+    <hyperlink ref="C30" r:id="rId28" xr:uid="{958760EB-2262-41C7-B971-6DB7AC4D2FDF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"No343. Integer Break finished"
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F01F013-12EA-4841-93D8-9B10BDC260FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DDE6F4-2F68-434C-A174-0A952757D8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -894,7 +894,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>注意一个因为dp考虑的分割数字至少有两个，状态转移还要考虑1个数字的情况；同时还可以用数学方法简化</t>
+    <t>注意一个因为dp考虑的分割数字至少有两个，状态转移还要考虑1个数字的情况；同时还可以用数学方法简化。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1522,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
"No583. Delete Operation for Two Strings finished"
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DDE6F4-2F68-434C-A174-0A952757D8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8036D9A9-65C4-4D89-9256-E2A7D535088B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="118">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -895,6 +895,22 @@
   </si>
   <si>
     <t>注意一个因为dp考虑的分割数字至少有两个，状态转移还要考虑1个数字的情况；同时还可以用数学方法简化。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>583. Delete Operation for Two Strings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/delete-operation-for-two-strings/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二维动态规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看出是要求最长公共子序列就很常规了</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1520,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2261,6 +2277,29 @@
         <v>113</v>
       </c>
       <c r="G31" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A32" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="10">
+        <v>44510</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="28" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2302,8 +2341,9 @@
     <hyperlink ref="C29" r:id="rId27" xr:uid="{DB5A1B9B-6195-4ED2-AE10-F30A38579E65}"/>
     <hyperlink ref="C30" r:id="rId28" xr:uid="{958760EB-2262-41C7-B971-6DB7AC4D2FDF}"/>
     <hyperlink ref="C31" r:id="rId29" xr:uid="{428978FF-68BA-436B-9338-02AEF9D1574F}"/>
+    <hyperlink ref="C32" r:id="rId30" xr:uid="{751373FB-14DC-469F-9A2D-1A8009D45A4F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId30"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
241. Different Ways to Add Parentheses finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8036D9A9-65C4-4D89-9256-E2A7D535088B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE2BA50-4CB6-4EDF-9D9A-20708819C3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="126">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -911,6 +911,37 @@
   </si>
   <si>
     <t>看出是要求最长公共子序列就很常规了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>204. Count Primes</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-primes/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>质数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>241. Different Ways to Add Parentheses</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/different-ways-to-add-parentheses/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按常规的一个个判断会超时，从奇数、开平方、倍数角度加快速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分治</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按操作符的位置进行分割dfs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1085,7 +1116,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1219,6 +1250,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1536,10 +1570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2301,6 +2335,58 @@
       </c>
       <c r="G32" s="28" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A33" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="20">
+        <v>44536</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A34" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="20">
+        <v>44537</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="G34" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="42" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2342,8 +2428,10 @@
     <hyperlink ref="C30" r:id="rId28" xr:uid="{958760EB-2262-41C7-B971-6DB7AC4D2FDF}"/>
     <hyperlink ref="C31" r:id="rId29" xr:uid="{428978FF-68BA-436B-9338-02AEF9D1574F}"/>
     <hyperlink ref="C32" r:id="rId30" xr:uid="{751373FB-14DC-469F-9A2D-1A8009D45A4F}"/>
+    <hyperlink ref="C33" r:id="rId31" xr:uid="{E6EBAC55-C6D1-4A83-915A-312EFF6422CC}"/>
+    <hyperlink ref="C34" r:id="rId32" xr:uid="{6C26FE61-F6AD-418D-9A12-744476DE19EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
README has modified and descriptions added
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE2BA50-4CB6-4EDF-9D9A-20708819C3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D36D2A-168F-4DDD-A31B-E78840B853B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="129">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -942,6 +942,18 @@
   </si>
   <si>
     <t>按操作符的位置进行分割dfs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No932. Beautiful Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/beautiful-array/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关键在于怎么把分解子问题，并利用奇偶性把子问题的结果线性增加合并为父问题的答案</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1249,10 +1261,10 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1570,10 +1582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1589,14 +1601,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
@@ -2356,7 +2368,7 @@
       <c r="F33" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="G33" s="45" t="s">
+      <c r="G33" s="44" t="s">
         <v>13</v>
       </c>
       <c r="H33" s="42" t="s">
@@ -2382,10 +2394,36 @@
       <c r="F34" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="G34" s="45" t="s">
+      <c r="G34" s="44" t="s">
         <v>13</v>
       </c>
       <c r="H34" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A35" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" s="20">
+        <v>44538</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="G35" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="42" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2430,8 +2468,9 @@
     <hyperlink ref="C32" r:id="rId30" xr:uid="{751373FB-14DC-469F-9A2D-1A8009D45A4F}"/>
     <hyperlink ref="C33" r:id="rId31" xr:uid="{E6EBAC55-C6D1-4A83-915A-312EFF6422CC}"/>
     <hyperlink ref="C34" r:id="rId32" xr:uid="{6C26FE61-F6AD-418D-9A12-744476DE19EC}"/>
+    <hyperlink ref="C35" r:id="rId33" xr:uid="{C0902AAE-3E08-410E-B656-A2631F84AE6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No312. Burst Balloons finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D36D2A-168F-4DDD-A31B-E78840B853B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EDD61C-C446-4E70-A01A-60C69031FD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="132">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -954,6 +954,18 @@
   </si>
   <si>
     <t>关键在于怎么把分解子问题，并利用奇偶性把子问题的结果线性增加合并为父问题的答案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No312. Burst Balloons</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/burst-balloons/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分治的依据是最后一个爆炸的元素为界，因为分治后的结果需要使用分治前的元素，所以需要构造比给定数组左右各多一个空位用于储存爆炸后左右位置的元素</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1582,10 +1594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2424,6 +2436,32 @@
         <v>13</v>
       </c>
       <c r="H35" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A36" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" s="16">
+        <v>44539</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="G36" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="42" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2469,8 +2507,9 @@
     <hyperlink ref="C33" r:id="rId31" xr:uid="{E6EBAC55-C6D1-4A83-915A-312EFF6422CC}"/>
     <hyperlink ref="C34" r:id="rId32" xr:uid="{6C26FE61-F6AD-418D-9A12-744476DE19EC}"/>
     <hyperlink ref="C35" r:id="rId33" xr:uid="{C0902AAE-3E08-410E-B656-A2631F84AE6F}"/>
+    <hyperlink ref="C36" r:id="rId34" xr:uid="{492586EA-1027-4200-B0B7-1A7565C2B6EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No415.415. Add Strings finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EDD61C-C446-4E70-A01A-60C69031FD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B534F039-9167-4FAC-A2E1-0449BD67E821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="142">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -966,6 +966,58 @@
   </si>
   <si>
     <t>分治的依据是最后一个爆炸的元素为界，因为分治后的结果需要使用分治前的元素，所以需要构造比给定数组左右各多一个空位用于储存爆炸后左右位置的元素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>504. Base 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/base-7/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单进制转换</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172. Factorial Trailing Zeroes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/factorial-trailing-zeroes/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>以下所有正整数某个特定质因数的个数求法</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>415. Add Strings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-strings/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串逐位相加；int和char的转换方法</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1594,10 +1646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2462,6 +2514,78 @@
         <v>13</v>
       </c>
       <c r="H36" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A37" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="6">
+        <v>44540</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="G37" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A38" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="10">
+        <v>44540</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G38" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A39" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" s="20">
+        <v>44542</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="G39" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="42" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2508,8 +2632,11 @@
     <hyperlink ref="C34" r:id="rId32" xr:uid="{6C26FE61-F6AD-418D-9A12-744476DE19EC}"/>
     <hyperlink ref="C35" r:id="rId33" xr:uid="{C0902AAE-3E08-410E-B656-A2631F84AE6F}"/>
     <hyperlink ref="C36" r:id="rId34" xr:uid="{492586EA-1027-4200-B0B7-1A7565C2B6EE}"/>
+    <hyperlink ref="C37" r:id="rId35" xr:uid="{F5E09882-71DE-4704-A6E4-0F2CD8642AAD}"/>
+    <hyperlink ref="C38" r:id="rId36" xr:uid="{E33162F0-9FB1-4510-AE41-69E422918BBC}"/>
+    <hyperlink ref="C39" r:id="rId37" xr:uid="{0324DD9A-BF32-419A-946F-DC4F2F811A4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No188. Best Time to Buy and Sell Stock IV finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B534F039-9167-4FAC-A2E1-0449BD67E821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056C2C9C-CA66-43CE-8347-BADA1703A855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="146">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1018,6 +1018,22 @@
   </si>
   <si>
     <t>字符串逐位相加；int和char的转换方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No188. Best Time to Buy and Sell Stock IV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-iv/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票交易</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分别用sell和buy两个数组表示第j次买入或者卖出的最大收益</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1646,10 +1662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2586,6 +2602,32 @@
         <v>13</v>
       </c>
       <c r="H39" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A40" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D40" s="16">
+        <v>44544</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="G40" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="42" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2635,8 +2677,9 @@
     <hyperlink ref="C37" r:id="rId35" xr:uid="{F5E09882-71DE-4704-A6E4-0F2CD8642AAD}"/>
     <hyperlink ref="C38" r:id="rId36" xr:uid="{E33162F0-9FB1-4510-AE41-69E422918BBC}"/>
     <hyperlink ref="C39" r:id="rId37" xr:uid="{0324DD9A-BF32-419A-946F-DC4F2F811A4E}"/>
+    <hyperlink ref="C40" r:id="rId38" xr:uid="{9A19D8E5-2A28-4C37-A9F0-78E4C5C01A76}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No309. Best Time to Buy and Sell Stock with Cooldown finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056C2C9C-CA66-43CE-8347-BADA1703A855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FB6D2B-CBED-4FCE-9E67-0B29D979F676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="150">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1034,6 +1034,22 @@
   </si>
   <si>
     <t>分别用sell和buy两个数组表示第j次买入或者卖出的最大收益</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>309. Best Time to Buy and Sell Stock with Cooldown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-with-cooldown/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票交易(状态机）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>涉及冷却时间的股票交易要用状态机</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1662,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2628,6 +2644,32 @@
         <v>13</v>
       </c>
       <c r="H40" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+      <c r="A41" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="20">
+        <v>44545</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F41" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G41" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="42" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2678,8 +2720,9 @@
     <hyperlink ref="C38" r:id="rId36" xr:uid="{E33162F0-9FB1-4510-AE41-69E422918BBC}"/>
     <hyperlink ref="C39" r:id="rId37" xr:uid="{0324DD9A-BF32-419A-946F-DC4F2F811A4E}"/>
     <hyperlink ref="C40" r:id="rId38" xr:uid="{9A19D8E5-2A28-4C37-A9F0-78E4C5C01A76}"/>
+    <hyperlink ref="C41" r:id="rId39" xr:uid="{C739E2E9-3F0E-43CC-8609-81BFCEF8B910}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId39"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No72. Edit Distance finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5FC91B-8A5B-4320-B9B8-BFBF3082264F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB18093-B2F1-4358-BCBB-52BD6089D8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="157">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1062,6 +1062,22 @@
   </si>
   <si>
     <t>带有交易费的股票交易，可以设置两个状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No72. Edit Distance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/edit-distance/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态规划，字符串编辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>和1143类似的dp数组设置，注意初始值设置</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1690,10 +1706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2280,8 +2296,8 @@
       <c r="F25" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="G25" s="28" t="s">
-        <v>37</v>
+      <c r="G25" s="28">
+        <v>44546</v>
       </c>
       <c r="H25" s="42" t="s">
         <v>94</v>
@@ -2705,6 +2721,29 @@
         <v>152</v>
       </c>
       <c r="G42" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A43" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D43" s="16">
+        <v>44546</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="G43" s="44" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2757,8 +2796,9 @@
     <hyperlink ref="C40" r:id="rId38" xr:uid="{9A19D8E5-2A28-4C37-A9F0-78E4C5C01A76}"/>
     <hyperlink ref="C41" r:id="rId39" xr:uid="{C739E2E9-3F0E-43CC-8609-81BFCEF8B910}"/>
     <hyperlink ref="C42" r:id="rId40" xr:uid="{BB68C324-FA08-47C6-BF35-A64743819E2B}"/>
+    <hyperlink ref="C43" r:id="rId41" xr:uid="{C688A64F-F13D-4B00-9B44-F74E326A7825}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId41"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No 650. 2 Keys Keyboard reviewed
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB18093-B2F1-4358-BCBB-52BD6089D8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86B2335-64F0-4D31-9EB0-04C4C6159FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="157">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1708,8 +1708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2397,8 +2397,8 @@
       <c r="F29" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="G29" s="28" t="s">
-        <v>37</v>
+      <c r="G29" s="28">
+        <v>44547</v>
       </c>
       <c r="H29" s="42" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
451. Sort Characters By Frequency reviewed
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86B2335-64F0-4D31-9EB0-04C4C6159FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD6E880-DF21-4A7C-92DE-10E6685FCDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="161">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1078,6 +1078,22 @@
   </si>
   <si>
     <t>和1143类似的dp数组设置，注意初始值设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>451. Sort Characters By Frequency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-characters-by-frequency/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桶排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arrays.sort重写comparator方法；注意不能传入基本数据类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1706,10 +1722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2745,6 +2761,35 @@
       </c>
       <c r="G43" s="44" t="s">
         <v>13</v>
+      </c>
+      <c r="H43" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A44" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44" s="20">
+        <v>44492</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="G44" s="28">
+        <v>44547</v>
+      </c>
+      <c r="H44" s="42" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2797,8 +2842,9 @@
     <hyperlink ref="C41" r:id="rId39" xr:uid="{C739E2E9-3F0E-43CC-8609-81BFCEF8B910}"/>
     <hyperlink ref="C42" r:id="rId40" xr:uid="{BB68C324-FA08-47C6-BF35-A64743819E2B}"/>
     <hyperlink ref="C43" r:id="rId41" xr:uid="{C688A64F-F13D-4B00-9B44-F74E326A7825}"/>
+    <hyperlink ref="C44" r:id="rId42" xr:uid="{379B8517-4C87-4D0B-A186-AF072F1B5EDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No10. Regular Expression Matching finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD6E880-DF21-4A7C-92DE-10E6685FCDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E57EB8-F167-4451-BE35-54C502243E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="164">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1094,6 +1094,46 @@
   </si>
   <si>
     <t>Arrays.sort重写comparator方法；注意不能传入基本数据类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10. Regular Expression Matching</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/regular-expression-matching/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分类讨论，关键就是带星号的情况下，是否要重复，状态转移方程不同；注意等价</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp[0][0]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>情况的初始化</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1268,7 +1308,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1406,6 +1446,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1722,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2789,6 +2832,32 @@
         <v>44547</v>
       </c>
       <c r="H44" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A45" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="16">
+        <v>44548</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F45" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="G45" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="42" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2843,8 +2912,9 @@
     <hyperlink ref="C42" r:id="rId40" xr:uid="{BB68C324-FA08-47C6-BF35-A64743819E2B}"/>
     <hyperlink ref="C43" r:id="rId41" xr:uid="{C688A64F-F13D-4B00-9B44-F74E326A7825}"/>
     <hyperlink ref="C44" r:id="rId42" xr:uid="{379B8517-4C87-4D0B-A186-AF072F1B5EDA}"/>
+    <hyperlink ref="C45" r:id="rId43" xr:uid="{BE7A3B23-931A-4D7A-92C6-1D9021EAD400}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId43"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
343. Integer Break and 53. Maximum Subarray reviewed
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E57EB8-F167-4451-BE35-54C502243E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE58716A-994A-41DC-AF3A-DAF0EA13A2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="164">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1141,7 +1141,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1258,6 +1258,14 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1308,7 +1316,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1444,11 +1452,14 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1767,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1784,14 +1795,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
@@ -2459,7 +2470,7 @@
       <c r="G29" s="28">
         <v>44547</v>
       </c>
-      <c r="H29" s="42" t="s">
+      <c r="H29" s="47" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2482,8 +2493,8 @@
       <c r="F30" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="G30" s="28" t="s">
-        <v>37</v>
+      <c r="G30" s="28">
+        <v>44548</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -2505,8 +2516,11 @@
       <c r="F31" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="G31" s="28" t="s">
-        <v>37</v>
+      <c r="G31" s="28">
+        <v>44548</v>
+      </c>
+      <c r="H31" s="42" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="42" x14ac:dyDescent="0.3">
@@ -2851,7 +2865,7 @@
       <c r="E45" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="F45" s="46" t="s">
+      <c r="F45" s="45" t="s">
         <v>163</v>
       </c>
       <c r="G45" s="44" t="s">

</xml_diff>

<commit_message>
No494. Target Sum finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE58716A-994A-41DC-AF3A-DAF0EA13A2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2521A5-5BA4-4C3B-A4BE-70782C1D4BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="168">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1134,6 +1134,50 @@
       </rPr>
       <t>情况的初始化</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>494. Target Sum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/target-sum/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>动态规划，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>背包</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怎样确定dp数组大小，负数情况怎么对应到下标</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1455,10 +1499,10 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1776,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1795,14 +1839,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
@@ -2470,7 +2514,7 @@
       <c r="G29" s="28">
         <v>44547</v>
       </c>
-      <c r="H29" s="47" t="s">
+      <c r="H29" s="46" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2873,6 +2917,29 @@
       </c>
       <c r="H45" s="42" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A46" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D46" s="20">
+        <v>44549</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="G46" s="44" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2927,8 +2994,9 @@
     <hyperlink ref="C43" r:id="rId41" xr:uid="{C688A64F-F13D-4B00-9B44-F74E326A7825}"/>
     <hyperlink ref="C44" r:id="rId42" xr:uid="{379B8517-4C87-4D0B-A186-AF072F1B5EDA}"/>
     <hyperlink ref="C45" r:id="rId43" xr:uid="{BE7A3B23-931A-4D7A-92C6-1D9021EAD400}"/>
+    <hyperlink ref="C46" r:id="rId44" xr:uid="{FCA0B21F-403E-4008-B156-9C1232F840F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId44"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No376. Wiggle Subsequence finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2521A5-5BA4-4C3B-A4BE-70782C1D4BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0218C76E-E03C-48B1-8B36-943B14C0AE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="172">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1178,6 +1178,59 @@
   </si>
   <si>
     <t>怎样确定dp数组大小，负数情况怎么对应到下标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>376. Wiggle Subsequence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/wiggle-subsequence/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态规划，摇摆序列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>纯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，数组要根据末尾两元素单调性分类；可以用贪心优化到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>O(n)</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1360,7 +1413,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1503,6 +1556,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1820,10 +1876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2940,6 +2996,32 @@
       </c>
       <c r="G46" s="44" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A47" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="D47" s="20">
+        <v>44551</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="G47" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="48" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2995,8 +3077,9 @@
     <hyperlink ref="C44" r:id="rId42" xr:uid="{379B8517-4C87-4D0B-A186-AF072F1B5EDA}"/>
     <hyperlink ref="C45" r:id="rId43" xr:uid="{BE7A3B23-931A-4D7A-92C6-1D9021EAD400}"/>
     <hyperlink ref="C46" r:id="rId44" xr:uid="{FCA0B21F-403E-4008-B156-9C1232F840F4}"/>
+    <hyperlink ref="C47" r:id="rId45" xr:uid="{8FC54213-4EFC-4E70-8B57-B1A1805CA8D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId45"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No241. Different Ways to Add Parentheses reviewed
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0218C76E-E03C-48B1-8B36-943B14C0AE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8876BFEB-2465-460B-845D-244FC69FCADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="172">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1555,10 +1555,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1878,8 +1878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1895,14 +1895,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
@@ -2691,8 +2691,8 @@
       <c r="F34" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="G34" s="44" t="s">
-        <v>13</v>
+      <c r="G34" s="44">
+        <v>44552</v>
       </c>
       <c r="H34" s="42" t="s">
         <v>94</v>
@@ -3020,7 +3020,7 @@
       <c r="G47" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="H47" s="48" t="s">
+      <c r="H47" s="47" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
No326. Power of Three finished and No312. Burst Balloons reviewed
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8876BFEB-2465-460B-845D-244FC69FCADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0334C2A2-A306-49EA-AEF1-A6DE2AE4E93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="175">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1231,6 +1231,18 @@
       </rPr>
       <t>O(n)</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>326. Power of Three</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/power-of-three/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意整数的范围</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1876,10 +1888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2743,8 +2755,8 @@
       <c r="F36" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="G36" s="44" t="s">
-        <v>13</v>
+      <c r="G36" s="44">
+        <v>44553</v>
       </c>
       <c r="H36" s="42" t="s">
         <v>94</v>
@@ -3022,6 +3034,29 @@
       </c>
       <c r="H47" s="47" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A48" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D48" s="6">
+        <v>44553</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="G48" s="44" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3078,8 +3113,9 @@
     <hyperlink ref="C45" r:id="rId43" xr:uid="{BE7A3B23-931A-4D7A-92C6-1D9021EAD400}"/>
     <hyperlink ref="C46" r:id="rId44" xr:uid="{FCA0B21F-403E-4008-B156-9C1232F840F4}"/>
     <hyperlink ref="C47" r:id="rId45" xr:uid="{8FC54213-4EFC-4E70-8B57-B1A1805CA8D1}"/>
+    <hyperlink ref="C48" r:id="rId46" xr:uid="{BDD5B583-9C8D-4A30-9FD5-646F288BD67D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No34 reviewed and No384. Shuffle an Array finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0334C2A2-A306-49EA-AEF1-A6DE2AE4E93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D9668C-FE00-4911-B75B-B11C387192CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="182">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1243,6 +1243,34 @@
   </si>
   <si>
     <t>注意整数的范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>384. Shuffle an Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/shuffle-an-array/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意本题考查洗牌算法，要求完全随机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>34. Find First and Last Position of Element in Sorted Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二分法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二分法找元素当存在多个元素时如何定位最小index和最大index；</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1888,10 +1916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3057,6 +3085,55 @@
       </c>
       <c r="G48" s="44" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A49" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" s="20">
+        <v>44554</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="G49" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+      <c r="A50" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D50" s="10">
+        <v>44468</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="G50" s="28">
+        <v>44554</v>
       </c>
     </row>
   </sheetData>
@@ -3114,8 +3191,10 @@
     <hyperlink ref="C46" r:id="rId44" xr:uid="{FCA0B21F-403E-4008-B156-9C1232F840F4}"/>
     <hyperlink ref="C47" r:id="rId45" xr:uid="{8FC54213-4EFC-4E70-8B57-B1A1805CA8D1}"/>
     <hyperlink ref="C48" r:id="rId46" xr:uid="{BDD5B583-9C8D-4A30-9FD5-646F288BD67D}"/>
+    <hyperlink ref="C49" r:id="rId47" xr:uid="{B261C574-E74C-4B63-9BEA-D04811C1C99A}"/>
+    <hyperlink ref="C50" r:id="rId48" xr:uid="{F3B108E9-68DA-418C-B00A-CC6A74498E9D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId47"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No528. Random Pick with Weight finished and No81 reviewed
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D9668C-FE00-4911-B75B-B11C387192CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36742B8E-9712-4719-A2EE-669E522BCDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="190">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1271,6 +1271,38 @@
   </si>
   <si>
     <t>二分法找元素当存在多个元素时如何定位最小index和最大index；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No528. Random Pick with Weight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/random-pick-with-weight/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学，随机选取</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学，带权重随机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利用前缀和实现带有权重的随机选取，注意random取随机数的范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>81. Search in Rotated Sorted Array II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-in-rotated-sorted-array-ii/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当数组中存在两个递增序列时，怎么判断mid位于哪个递增序列中</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1916,10 +1948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3101,7 +3133,7 @@
         <v>44554</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="F49" s="21" t="s">
         <v>177</v>
@@ -3134,6 +3166,55 @@
       </c>
       <c r="G50" s="28">
         <v>44554</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A51" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="D51" s="20">
+        <v>44555</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="G51" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A52" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D52" s="10">
+        <v>44472</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="G52" s="28">
+        <v>44555</v>
       </c>
     </row>
   </sheetData>
@@ -3193,8 +3274,10 @@
     <hyperlink ref="C48" r:id="rId46" xr:uid="{BDD5B583-9C8D-4A30-9FD5-646F288BD67D}"/>
     <hyperlink ref="C49" r:id="rId47" xr:uid="{B261C574-E74C-4B63-9BEA-D04811C1C99A}"/>
     <hyperlink ref="C50" r:id="rId48" xr:uid="{F3B108E9-68DA-418C-B00A-CC6A74498E9D}"/>
+    <hyperlink ref="C51" r:id="rId49" xr:uid="{1DEF0DDC-7988-496B-86A4-105B8F57517B}"/>
+    <hyperlink ref="C52" r:id="rId50" xr:uid="{2224D218-DFD9-42AC-8A5A-374C06CA6769}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId49"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId51"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No382. Linked List Random Node finished and No154 reviewed
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36742B8E-9712-4719-A2EE-669E522BCDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BB1D3D-6FA2-44C5-A28D-0E78CBD3D11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="197">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1303,6 +1303,46 @@
   </si>
   <si>
     <t>当数组中存在两个递增序列时，怎么判断mid位于哪个递增序列中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>382. Linked List Random Node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-random-node/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学，水库算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水库算法，在事先不知道数组大小的情况下遍历做到随机选取元素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>154. Find Minimum in Rotated Sorted Array II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-minimum-in-rotated-sorted-array-ii/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rotate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数组找最值</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1948,10 +1988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3215,6 +3255,55 @@
       </c>
       <c r="G52" s="28">
         <v>44555</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A53" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="D53" s="20">
+        <v>44556</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="G53" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+      <c r="A54" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="D54" s="20">
+        <v>44470</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="G54" s="28">
+        <v>44556</v>
       </c>
     </row>
   </sheetData>
@@ -3276,8 +3365,10 @@
     <hyperlink ref="C50" r:id="rId48" xr:uid="{F3B108E9-68DA-418C-B00A-CC6A74498E9D}"/>
     <hyperlink ref="C51" r:id="rId49" xr:uid="{1DEF0DDC-7988-496B-86A4-105B8F57517B}"/>
     <hyperlink ref="C52" r:id="rId50" xr:uid="{2224D218-DFD9-42AC-8A5A-374C06CA6769}"/>
+    <hyperlink ref="C53" r:id="rId51" xr:uid="{581FBECE-7E00-470D-9FC1-393F8CFAAFD1}"/>
+    <hyperlink ref="C54" r:id="rId52" xr:uid="{798EE8DF-9CA4-47FA-8328-71E3BEEA462B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId51"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId53"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No67 and No 168 finished and No540 reviewed
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BB1D3D-6FA2-44C5-A28D-0E78CBD3D11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DCF192-0CE8-4954-907C-E2F1DF6CFF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="209">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1343,6 +1343,66 @@
       </rPr>
       <t>数组找最值</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>168. Excel Sheet Column Title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/excel-sheet-column-title/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学，进制转化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意进制起始位的细节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>67. Add Binary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-binary/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学，字符串加法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>StringBuffer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>翻转函数；长度不同时按位相加的写法</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>540. Single Element in a Sorted Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/single-element-in-a-sorted-array/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奇数长度数组，mid左右元素个数相同；通过mid和mid+1元素比较锁定单个元素位置在左边还是右边</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1988,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3304,6 +3364,78 @@
       </c>
       <c r="G54" s="28">
         <v>44556</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A55" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="D55" s="6">
+        <v>44558</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="F55" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="G55" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A56" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D56" s="6">
+        <v>44558</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G56" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A57" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D57" s="20">
+        <v>44470</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="F57" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="G57" s="28">
+        <v>44558</v>
+      </c>
+      <c r="H57" s="42" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3367,8 +3499,11 @@
     <hyperlink ref="C52" r:id="rId50" xr:uid="{2224D218-DFD9-42AC-8A5A-374C06CA6769}"/>
     <hyperlink ref="C53" r:id="rId51" xr:uid="{581FBECE-7E00-470D-9FC1-393F8CFAAFD1}"/>
     <hyperlink ref="C54" r:id="rId52" xr:uid="{798EE8DF-9CA4-47FA-8328-71E3BEEA462B}"/>
+    <hyperlink ref="C55" r:id="rId53" xr:uid="{B493A519-C6E4-4603-9EAC-0C4CCB4ACF1C}"/>
+    <hyperlink ref="C56" r:id="rId54" xr:uid="{1EC5AF8B-42BD-48AA-BDFB-0BD2252218C8}"/>
+    <hyperlink ref="C57" r:id="rId55" xr:uid="{5969152C-B531-45C4-9E83-CE3E83F34337}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId53"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId56"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No238. Product of Array Except Self finished and No135 Candy reviewed
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DCF192-0CE8-4954-907C-E2F1DF6CFF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3503CAE1-739D-45E2-BD8D-92643E1A9C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="216">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1403,6 +1403,90 @@
   </si>
   <si>
     <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>238. Product of Array Except Self</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/product-of-array-except-self/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>类似于分糖果的思路，从左到右遍历一遍，然后再从右往左遍历一遍，记录乘积</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>product</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，先更新</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ans</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，再更新</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>product</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>135. Candy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/candy/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贪心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从左往右遍历使每个元素与相邻右元素满足要求；从右往左遍历使与相邻做元素满足要求</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2048,10 +2132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3436,6 +3520,52 @@
       </c>
       <c r="H57" s="42" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A58" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D58" s="10">
+        <v>44559</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G58" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A59" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="D59" s="20">
+        <v>44442</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="F59" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="G59" s="28">
+        <v>44559</v>
       </c>
     </row>
   </sheetData>
@@ -3502,8 +3632,10 @@
     <hyperlink ref="C55" r:id="rId53" xr:uid="{B493A519-C6E4-4603-9EAC-0C4CCB4ACF1C}"/>
     <hyperlink ref="C56" r:id="rId54" xr:uid="{1EC5AF8B-42BD-48AA-BDFB-0BD2252218C8}"/>
     <hyperlink ref="C57" r:id="rId55" xr:uid="{5969152C-B531-45C4-9E83-CE3E83F34337}"/>
+    <hyperlink ref="C58" r:id="rId56" xr:uid="{1B7E8ED9-ED88-4E02-AB7B-563395122D6C}"/>
+    <hyperlink ref="C59" r:id="rId57" xr:uid="{F3A448BE-449A-45D1-8086-D5239D3D6F99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId56"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId58"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No462. Minimum Moves to Equal Array Elements II finished and No122 reviewed
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3503CAE1-739D-45E2-BD8D-92643E1A9C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329070C0-D8D2-464A-95D2-2A5E674120F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="223">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1487,6 +1487,62 @@
   </si>
   <si>
     <t>从左往右遍历使每个元素与相邻右元素满足要求；从右往左遍历使与相邻做元素满足要求</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>462. Minimum Moves to Equal Array Elements II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-moves-to-equal-array-elements-ii/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>类似找类似于求</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>|x-1|+|x-2|+...+||x-n|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的最小值</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>122. Best Time to Buy and Sell Stock II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-ii/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贪心，股票交易</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有交易费、冷却天数的股票交易，直接谷底买进，谷峰卖出即可</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2132,10 +2188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3566,6 +3622,55 @@
       </c>
       <c r="G59" s="28">
         <v>44559</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+      <c r="A60" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="D60" s="20">
+        <v>44560</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="F60" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="G60" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A61" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="D61" s="6">
+        <v>44458</v>
+      </c>
+      <c r="E61" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="F61" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="G61" s="28">
+        <v>44560</v>
       </c>
     </row>
   </sheetData>
@@ -3634,8 +3739,10 @@
     <hyperlink ref="C57" r:id="rId55" xr:uid="{5969152C-B531-45C4-9E83-CE3E83F34337}"/>
     <hyperlink ref="C58" r:id="rId56" xr:uid="{1B7E8ED9-ED88-4E02-AB7B-563395122D6C}"/>
     <hyperlink ref="C59" r:id="rId57" xr:uid="{F3A448BE-449A-45D1-8086-D5239D3D6F99}"/>
+    <hyperlink ref="C60" r:id="rId58" xr:uid="{8DF5F84A-BDAB-42E9-805B-0E331249D704}"/>
+    <hyperlink ref="C61" r:id="rId59" xr:uid="{92FFBCB8-2E3B-4C4E-AC39-3AF8457FE058}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId58"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId60"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No4 reviewed and No169 finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329070C0-D8D2-464A-95D2-2A5E674120F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6EAC55-9095-4D57-8CE0-5967D02AFD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="230">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1543,6 +1543,34 @@
   </si>
   <si>
     <t>没有交易费、冷却天数的股票交易，直接谷底买进，谷峰卖出即可</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. Median of Two Sorted Arrays</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/median-of-two-sorted-arrays/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二分法，合并数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>两个有序数组合并求中位数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>169. Majority Element</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/majority-element/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怎样快速找到最多的元素</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1550,7 +1578,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1675,6 +1703,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1725,7 +1760,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1871,6 +1906,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2188,10 +2226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3671,6 +3709,55 @@
       </c>
       <c r="G61" s="28">
         <v>44560</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A62" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="D62" s="16">
+        <v>44471</v>
+      </c>
+      <c r="E62" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="G62" s="28">
+        <v>44567</v>
+      </c>
+      <c r="H62" s="49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D63" s="10">
+        <v>44566</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="G63" s="44" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3741,8 +3828,10 @@
     <hyperlink ref="C59" r:id="rId57" xr:uid="{F3A448BE-449A-45D1-8086-D5239D3D6F99}"/>
     <hyperlink ref="C60" r:id="rId58" xr:uid="{8DF5F84A-BDAB-42E9-805B-0E331249D704}"/>
     <hyperlink ref="C61" r:id="rId59" xr:uid="{92FFBCB8-2E3B-4C4E-AC39-3AF8457FE058}"/>
+    <hyperlink ref="C62" r:id="rId60" xr:uid="{758C40D5-9342-4794-9D98-360C44C31C96}"/>
+    <hyperlink ref="C63" r:id="rId61" xr:uid="{F0BF4722-23CF-45B2-89A1-238278D1C85C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId60"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId62"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bitwise operation four topics added
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6EAC55-9095-4D57-8CE0-5967D02AFD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EB11D6-4DBC-4920-A8C4-8A615324682B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="249">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1571,6 +1571,110 @@
   </si>
   <si>
     <t>怎样快速找到最多的元素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>202. Happy Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/happy-number/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类似快慢指针找环路可以把空间复杂度降到1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>470. Implement Rand10() Using Rand7()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-rand10-using-rand7/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用一个随机生成器生成一个更大范围的随机生成器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>342. Power of Four</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/power-of-four/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位运算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>136. Single Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>判断2的次幂n&amp;(n-1)==0,4的次幂就多加一个奇数位的条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/single-number/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>用到了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0&amp;x=x,x&amp;x=0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的技巧</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>190. Reverse Bits</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-bits/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>和1与获取末位然后结果移位后或运算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>318. Maximum Product of Word Lengths</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-product-of-word-lengths/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用一个26位的二进制数字储存马哥字符串中字母的出现情况</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1905,10 +2009,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2226,17 +2330,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.58203125" style="7"/>
-    <col min="2" max="2" width="20.58203125" style="2"/>
-    <col min="3" max="3" width="20.58203125" style="7"/>
+    <col min="2" max="2" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.25" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="20.58203125" style="2"/>
     <col min="6" max="6" width="64.58203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="20.58203125" style="28"/>
@@ -2245,14 +2349,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
@@ -3266,10 +3370,10 @@
       <c r="F43" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="G43" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="42" t="s">
+      <c r="G43" s="28">
+        <v>44206</v>
+      </c>
+      <c r="H43" s="46" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3733,7 +3837,7 @@
       <c r="G62" s="28">
         <v>44567</v>
       </c>
-      <c r="H62" s="49" t="s">
+      <c r="H62" s="48" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3758,6 +3862,154 @@
       </c>
       <c r="G63" s="44" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A64" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D64" s="10">
+        <v>44569</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="G64" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A65" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D65" s="10">
+        <v>44569</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="G65" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A66" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="D66" s="10">
+        <v>44571</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G66" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H66" s="47"/>
+    </row>
+    <row r="67" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A67" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="D67" s="10">
+        <v>44571</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F67" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="G67" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H67" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A68" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D68" s="10">
+        <v>44571</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F68" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="G68" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+      <c r="A69" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D69" s="10">
+        <v>44572</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="G69" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H69" s="47" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3830,8 +4082,14 @@
     <hyperlink ref="C61" r:id="rId59" xr:uid="{92FFBCB8-2E3B-4C4E-AC39-3AF8457FE058}"/>
     <hyperlink ref="C62" r:id="rId60" xr:uid="{758C40D5-9342-4794-9D98-360C44C31C96}"/>
     <hyperlink ref="C63" r:id="rId61" xr:uid="{F0BF4722-23CF-45B2-89A1-238278D1C85C}"/>
+    <hyperlink ref="C64" r:id="rId62" xr:uid="{88480C3B-E81B-4F06-9206-EE98324F78A4}"/>
+    <hyperlink ref="C65" r:id="rId63" xr:uid="{CED9DD03-87CF-4824-B0FA-7E2ED74E4171}"/>
+    <hyperlink ref="C66" r:id="rId64" xr:uid="{35AA5279-BECA-40A3-BFEE-AE199E3280FA}"/>
+    <hyperlink ref="C67" r:id="rId65" xr:uid="{0B2A9B82-5A61-4550-9C93-E361B6C184F0}"/>
+    <hyperlink ref="C68" r:id="rId66" xr:uid="{457C80A6-85E0-465E-B7F8-148A34DBFA25}"/>
+    <hyperlink ref="C69" r:id="rId67" xr:uid="{C82E8BD2-AC04-411D-B4E1-4930793ED920}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId62"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId68"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No260 and No476 finished and No693 reviewed
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EB11D6-4DBC-4920-A8C4-8A615324682B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23EAA73-D9CB-42E3-9969-BEB4E0E1E65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="257">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1674,7 +1674,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>用一个26位的二进制数字储存马哥字符串中字母的出现情况</t>
+    <t>476. Number Complement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-complement/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用一个26位的二进制数字储存每个字符串中字母的出现情况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>190</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的变种题，获取末位元素后和1异或</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>693. Binary Number with Alternating Bits</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/single-number-iii/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>想办法获取111…111和1000...000这两种数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>260. Single Number III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>136</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的升级版，需要思考怎么把数组分为两部分，两个单个数分开，然后两部分分别异或</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2330,10 +2386,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2386,7 +2444,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>47</v>
       </c>
@@ -2409,7 +2467,7 @@
         <v>44499</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>51</v>
       </c>
@@ -2432,7 +2490,7 @@
         <v>44499</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
         <v>53</v>
       </c>
@@ -2645,7 +2703,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A14" s="34" t="s">
         <v>18</v>
       </c>
@@ -2691,7 +2749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
         <v>26</v>
       </c>
@@ -2737,7 +2795,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>32</v>
       </c>
@@ -2878,7 +2936,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>83</v>
       </c>
@@ -2901,7 +2959,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A25" s="34" t="s">
         <v>86</v>
       </c>
@@ -2927,7 +2985,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A26" s="34" t="s">
         <v>89</v>
       </c>
@@ -3028,7 +3086,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A30" s="32" t="s">
         <v>106</v>
       </c>
@@ -3077,7 +3135,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
         <v>114</v>
       </c>
@@ -3126,7 +3184,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A34" s="34" t="s">
         <v>121</v>
       </c>
@@ -3227,7 +3285,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A38" s="27" t="s">
         <v>136</v>
       </c>
@@ -3276,7 +3334,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A40" s="33" t="s">
         <v>142</v>
       </c>
@@ -3302,7 +3360,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A41" s="34" t="s">
         <v>146</v>
       </c>
@@ -3328,7 +3386,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
         <v>150</v>
       </c>
@@ -3377,7 +3435,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A44" s="34" t="s">
         <v>157</v>
       </c>
@@ -3403,7 +3461,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A45" s="33" t="s">
         <v>161</v>
       </c>
@@ -3452,7 +3510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A47" s="34" t="s">
         <v>168</v>
       </c>
@@ -3527,7 +3585,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
         <v>178</v>
       </c>
@@ -3550,7 +3608,7 @@
         <v>44554</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A51" s="34" t="s">
         <v>182</v>
       </c>
@@ -3576,7 +3634,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A52" s="27" t="s">
         <v>187</v>
       </c>
@@ -3599,7 +3657,7 @@
         <v>44555</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A53" s="34" t="s">
         <v>190</v>
       </c>
@@ -3625,7 +3683,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A54" s="34" t="s">
         <v>194</v>
       </c>
@@ -3648,7 +3706,7 @@
         <v>44556</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A55" s="32" t="s">
         <v>197</v>
       </c>
@@ -3694,7 +3752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A57" s="34" t="s">
         <v>205</v>
       </c>
@@ -3720,7 +3778,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A58" s="27" t="s">
         <v>209</v>
       </c>
@@ -3766,7 +3824,7 @@
         <v>44559</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A60" s="34" t="s">
         <v>216</v>
       </c>
@@ -3792,7 +3850,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A61" s="32" t="s">
         <v>219</v>
       </c>
@@ -3815,7 +3873,7 @@
         <v>44560</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A62" s="33" t="s">
         <v>223</v>
       </c>
@@ -3887,7 +3945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A65" s="27" t="s">
         <v>233</v>
       </c>
@@ -3986,7 +4044,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A69" s="27" t="s">
         <v>246</v>
       </c>
@@ -4003,12 +4061,84 @@
         <v>238</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G69" s="44" t="s">
         <v>13</v>
       </c>
       <c r="H69" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A70" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="D70" s="10">
+        <v>44573</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="G70" s="28">
+        <v>44574</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A71" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="D71" s="6">
+        <v>44574</v>
+      </c>
+      <c r="E71" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="G71" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="A72" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D72" s="20">
+        <v>44574</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="F72" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="G72" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H72" s="47" t="s">
         <v>94</v>
       </c>
     </row>
@@ -4088,8 +4218,11 @@
     <hyperlink ref="C67" r:id="rId65" xr:uid="{0B2A9B82-5A61-4550-9C93-E361B6C184F0}"/>
     <hyperlink ref="C68" r:id="rId66" xr:uid="{457C80A6-85E0-465E-B7F8-148A34DBFA25}"/>
     <hyperlink ref="C69" r:id="rId67" xr:uid="{C82E8BD2-AC04-411D-B4E1-4930793ED920}"/>
+    <hyperlink ref="C71" r:id="rId68" xr:uid="{C7724BD6-72C9-4184-8F29-1E5D5103CBDE}"/>
+    <hyperlink ref="C72" r:id="rId69" xr:uid="{4E0EF049-DD87-4D1F-BD6D-F38FF4C76E43}"/>
+    <hyperlink ref="C70" r:id="rId70" xr:uid="{DC0EDF97-6A43-4C03-9F8B-7B2426BF1109}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId68"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId71"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No23 218 239 1 finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23EAA73-D9CB-42E3-9969-BEB4E0E1E65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3BA5D0-06DB-4835-BACA-2F8F0B34B7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="305">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1731,6 +1731,264 @@
       </rPr>
       <t>的升级版，需要思考怎么把数组分为两部分，两个单个数分开，然后两部分分别异或</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>448. Find All Numbers Disappeared in an Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-all-numbers-disappeared-in-an-array/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单两次遍历数组即可</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>48. Rotate Image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotate-image/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组旋转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组原地旋转，注意旋转后的坐标关系，以及不要重复旋转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>240. Search a 2D Matrix II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-a-2d-matrix-ii/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组，寻找元素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在行、列有序的二维数组中寻找元素的技巧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>769. Max Chunks To Make Sorted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/max-chunks-to-make-sorted/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>题目等价于找到最小的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>使得</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>A[:k+1]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>包含</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0~k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的所有元素</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>232. Implement Queue using Stacks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-queue-using-stacks/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经典用两个栈来实现先入先出队列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>155. Min Stack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/min-stack/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在常数时间复杂度获取栈的最小值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20. Valid Parentheses</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-parentheses/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栈，括号匹配</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>除了匹配以外，不要遗漏括号多余的情况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>739. Daily Temperatures</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/daily-temperatures/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单调栈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按温度递减顺序，将入栈顺序压栈，出栈时序号之差即为等待天数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>239. Sliding Window Maximum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23. Merge k Sorted Lists</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-k-sorted-lists/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优先队列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将所有的list的节点加入优先队列，每次取出的值就是最小值，这样就达到了排序的效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>218. The Skyline Problem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/the-skyline-problem/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>找到所有高度变化的第一个点，按节点的顺序加入或弹出优先队列，若所有节点中的最大高度变化了说明加入起始节点或者弹出末尾节点后是转折点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sliding-window-maximum/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>双端队列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单调栈的变种题，注意入队的是数组下标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Two Sum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/two-sum/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈希</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>遍历到num时查看target-num的哈希是否存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>128. Longest Consecutive Sequence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-consecutive-sequence/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放入set后向左向右遍历的同时删除元素</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2386,12 +2644,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4140,6 +4398,318 @@
       </c>
       <c r="H72" s="47" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A73" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="D73" s="6">
+        <v>44575</v>
+      </c>
+      <c r="E73" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="F73" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="G73" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A74" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="D74" s="10">
+        <v>44575</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="G74" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A75" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="D75" s="10">
+        <v>44576</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="G75" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A76" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="D76" s="10">
+        <v>44577</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="F76" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="G76" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A77" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="D77" s="6">
+        <v>44578</v>
+      </c>
+      <c r="E77" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="F77" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="G77" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A78" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D78" s="10">
+        <v>44579</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="F78" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="G78" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H78" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A79" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="D79" s="6">
+        <v>44580</v>
+      </c>
+      <c r="E79" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="F79" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="G79" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A80" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="D80" s="20">
+        <v>44581</v>
+      </c>
+      <c r="E80" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="F80" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="G80" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H80" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A81" s="33" t="s">
+        <v>288</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="D81" s="16">
+        <v>44582</v>
+      </c>
+      <c r="E81" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="F81" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="G81" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H81" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A82" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="B82" s="14"/>
+      <c r="C82" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="D82" s="16">
+        <v>44583</v>
+      </c>
+      <c r="E82" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="F82" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="G82" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H82" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A83" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="D83" s="16">
+        <v>44584</v>
+      </c>
+      <c r="E83" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="F83" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="G83" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H83" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A84" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="D84" s="6">
+        <v>44585</v>
+      </c>
+      <c r="E84" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="F84" s="23" t="s">
+        <v>301</v>
+      </c>
+      <c r="G84" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A85" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="D85" s="20">
+        <v>44585</v>
+      </c>
+      <c r="E85" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="F85" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="G85" s="44" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -4221,8 +4791,21 @@
     <hyperlink ref="C71" r:id="rId68" xr:uid="{C7724BD6-72C9-4184-8F29-1E5D5103CBDE}"/>
     <hyperlink ref="C72" r:id="rId69" xr:uid="{4E0EF049-DD87-4D1F-BD6D-F38FF4C76E43}"/>
     <hyperlink ref="C70" r:id="rId70" xr:uid="{DC0EDF97-6A43-4C03-9F8B-7B2426BF1109}"/>
+    <hyperlink ref="C73" r:id="rId71" xr:uid="{D9FA43CC-01C1-4E04-84FA-E6100E601BC5}"/>
+    <hyperlink ref="C74" r:id="rId72" xr:uid="{80633123-96DF-4FFC-B196-196409A7D706}"/>
+    <hyperlink ref="C75" r:id="rId73" xr:uid="{423E76C4-6D74-4BB6-A352-F36202E7ACAB}"/>
+    <hyperlink ref="C76" r:id="rId74" xr:uid="{D7AD8363-BA8E-4C53-8C7D-FF252CD1B5F5}"/>
+    <hyperlink ref="C77" r:id="rId75" xr:uid="{5098184E-631E-496D-BE62-8CC29327E30A}"/>
+    <hyperlink ref="C78" r:id="rId76" xr:uid="{8A6FD2C6-806D-4478-B1DD-477686430C69}"/>
+    <hyperlink ref="C79" r:id="rId77" xr:uid="{AD10A2D5-C381-4B0B-945A-850F3EA2C966}"/>
+    <hyperlink ref="C80" r:id="rId78" xr:uid="{5197DA3F-3F98-47C8-8F95-822B4FD410AE}"/>
+    <hyperlink ref="C81" r:id="rId79" xr:uid="{A2C9FC91-35D8-4136-85E7-F56BD742E86C}"/>
+    <hyperlink ref="C82" r:id="rId80" xr:uid="{794331CA-6947-43E7-A1F7-A550B35037F1}"/>
+    <hyperlink ref="C83" r:id="rId81" xr:uid="{E753B962-4BC6-4367-BB27-C86C3E02B1E8}"/>
+    <hyperlink ref="C84" r:id="rId82" xr:uid="{756DE8B6-B460-4DBE-B768-22586237C0BF}"/>
+    <hyperlink ref="C85" r:id="rId83" xr:uid="{2CDD0CEB-CA4F-48A8-9242-CEF04AD3E034}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId71"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId84"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No 566 225 503 332 302 149 finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3BA5D0-06DB-4835-BACA-2F8F0B34B7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382F1585-C82E-4F35-AB95-88148199BE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="334">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1989,6 +1989,134 @@
   </si>
   <si>
     <t>放入set后向左向右遍历的同时删除元素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>149. Max Points on a Line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/max-points-on-a-line/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意相同点和斜率不存在的情况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>332. Reconstruct Itinerary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reconstruct-itinerary/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈希，栈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用哈希记录站点之间的关系（一对多），用栈来依次弹出最后一个站点，注意一对多的关系入栈按字母序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>303. Range Sum Query - Immutable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/range-sum-query-immutable/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组，前缀和</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利用前缀和数组来计算固定区间的子序列之和</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>304. Range Sum Query 2D - Immutable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/range-sum-query-2d-immutable/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>积分和，动态规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是算矩形形区域元素和的动态规划变种，由一点确定矩形变为两点确定矩形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>560. Subarray Sum Equals K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subarray-sum-equals-k/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈希，动态规划，前缀和</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记录前缀和为psum的情况，每次计算新的psum，检查psum-k的哈希值更新当前满足k的子序列个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>566. Reshape the Matrix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reshape-the-matrix/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意换行部分的细节即可</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>225. Implement Stack using Queues</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-stack-using-queues/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>队列，栈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利用队列实现栈，主要就是元素在两个队列之间流动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>503. Next Greater Element II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/next-greater-element-ii/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>739</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的变种，由于是循环数组，整个数组需要循环两遍</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2644,12 +2772,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
+      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4709,6 +4837,199 @@
         <v>304</v>
       </c>
       <c r="G85" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A86" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="D86" s="16">
+        <v>44587</v>
+      </c>
+      <c r="E86" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="F86" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="G86" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H86" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A87" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="D87" s="16">
+        <v>44588</v>
+      </c>
+      <c r="E87" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="F87" s="35" t="s">
+        <v>311</v>
+      </c>
+      <c r="G87" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H87" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A88" s="32" t="s">
+        <v>312</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="D88" s="6">
+        <v>44589</v>
+      </c>
+      <c r="E88" s="23" t="s">
+        <v>314</v>
+      </c>
+      <c r="F88" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="G88" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A89" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="B89" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="D89" s="20">
+        <v>44589</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="F89" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="G89" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A90" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="B90" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="D90" s="20">
+        <v>44589</v>
+      </c>
+      <c r="E90" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="F90" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="G90" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A91" s="32" t="s">
+        <v>324</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="D91" s="6">
+        <v>44590</v>
+      </c>
+      <c r="E91" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="F91" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="G91" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A92" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="D92" s="6">
+        <v>44590</v>
+      </c>
+      <c r="E92" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="F92" s="23" t="s">
+        <v>330</v>
+      </c>
+      <c r="G92" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A93" s="34" t="s">
+        <v>331</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="D93" s="20">
+        <v>44590</v>
+      </c>
+      <c r="E93" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="F93" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="G93" s="44" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4804,8 +5125,16 @@
     <hyperlink ref="C83" r:id="rId81" xr:uid="{E753B962-4BC6-4367-BB27-C86C3E02B1E8}"/>
     <hyperlink ref="C84" r:id="rId82" xr:uid="{756DE8B6-B460-4DBE-B768-22586237C0BF}"/>
     <hyperlink ref="C85" r:id="rId83" xr:uid="{2CDD0CEB-CA4F-48A8-9242-CEF04AD3E034}"/>
+    <hyperlink ref="C86" r:id="rId84" xr:uid="{5C9F1471-809C-4F31-9CE7-2864C4BB7C59}"/>
+    <hyperlink ref="C87" r:id="rId85" xr:uid="{5B4004A6-16D2-4ADE-98FA-B1A006AE1684}"/>
+    <hyperlink ref="C88" r:id="rId86" xr:uid="{25EB30E2-5B31-4F0E-905F-5C25EB8CE3E2}"/>
+    <hyperlink ref="C89" r:id="rId87" xr:uid="{9790A5AB-1690-48D5-B087-9774D46E13CC}"/>
+    <hyperlink ref="C90" r:id="rId88" xr:uid="{6D843575-5BFB-4825-BED7-D09C486BCFBB}"/>
+    <hyperlink ref="C91" r:id="rId89" xr:uid="{991D402B-69D3-4402-9AD1-2E94B919F915}"/>
+    <hyperlink ref="C92" r:id="rId90" xr:uid="{D752215C-AC3C-447B-A9B9-A5DEBAE51CB2}"/>
+    <hyperlink ref="C93" r:id="rId91" xr:uid="{95E2579D-C9AF-44CF-B1BA-DB25334A31DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId84"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId92"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No 217 697 594 finished
</commit_message>
<xml_diff>
--- a/Leetcode_excel/leetcode_everyday .xlsx
+++ b/Leetcode_excel/leetcode_everyday .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CS\Leetcode\leetcode_101-master\Leetcode_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382F1585-C82E-4F35-AB95-88148199BE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D924100D-2542-4EBF-9EA2-4094AE024BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4745762B-DB5C-4821-8836-735B7687E9EC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="343">
   <si>
     <t>257. Binary Tree Paths</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2117,6 +2117,41 @@
       </rPr>
       <t>的变种，由于是循环数组，整个数组需要循环两遍</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>217. Contains Duplicate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/contains-duplicate/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单用set查重即可</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>697. Degree of an Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/degree-of-an-array/</t>
+  </si>
+  <si>
+    <t>hash需要记录两个数据，一个是出现的次数，一个是序列的长度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>594. Longest Harmonious Subsequence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-harmonious-subsequence/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关键就是最后的序列里面只有相邻的两个值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2772,12 +2807,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34E4F9-F957-41ED-BEB0-488A13FD91EE}">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
+      <selection pane="bottomLeft" activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5031,6 +5066,78 @@
       </c>
       <c r="G93" s="44" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A94" s="32" t="s">
+        <v>334</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="D94" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E94" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="F94" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="G94" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A95" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="D95" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E95" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="F95" s="23" t="s">
+        <v>339</v>
+      </c>
+      <c r="G95" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A96" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="D96" s="10">
+        <v>44591</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="F96" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="G96" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H96" s="47" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -5133,8 +5240,11 @@
     <hyperlink ref="C91" r:id="rId89" xr:uid="{991D402B-69D3-4402-9AD1-2E94B919F915}"/>
     <hyperlink ref="C92" r:id="rId90" xr:uid="{D752215C-AC3C-447B-A9B9-A5DEBAE51CB2}"/>
     <hyperlink ref="C93" r:id="rId91" xr:uid="{95E2579D-C9AF-44CF-B1BA-DB25334A31DE}"/>
+    <hyperlink ref="C94" r:id="rId92" xr:uid="{9456C26A-81AA-4061-AEDC-0D86452BC25B}"/>
+    <hyperlink ref="C95" r:id="rId93" xr:uid="{A0C3CE47-BE79-405E-8CD4-E4CA7B5F16F6}"/>
+    <hyperlink ref="C96" r:id="rId94" xr:uid="{99078CCF-ACC7-4AB3-BCD0-C127B2A86006}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId92"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId95"/>
 </worksheet>
 </file>
</xml_diff>